<commit_message>
Hyperlinks created through HYPERLINK formula function do not register hyperlink to the worksheet. The links created by formula didn't work and the addition of the hyperlink to the cell caused an exception when the formula was evaluated during save.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Misc/Hyperlinks.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Misc/Hyperlinks.xlsx
@@ -428,7 +428,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:A14"/>
+  <x:dimension ref="A1:A16"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -493,23 +493,32 @@
       </x:c>
     </x:row>
     <x:row r="12" spans="1:1">
-      <x:c r="A12" s="1">
-        <x:f>HYPERLINK("mailto:test@test.com", "Send Email")</x:f>
+      <x:c r="A12" s="0">
+        <x:f>HYPERLINK("mailto:test@test.com", "Send Email through formula")</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:1">
+      <x:c r="A13" s="0">
+        <x:f>HYPERLINK("[Hyperlinks.xlsx]Hyperlinks!B2:C4", "Link to range through formula")</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:1">
+      <x:c r="A14" s="0">
+        <x:f>HYPERLINK("[../Test.xlsx]Sheet1!B2:C4", "Link to another file through formula")</x:f>
       </x:c>
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="A1" r:id="rId14"/>
-    <x:hyperlink ref="A2" r:id="rId15" tooltip="Click to go to Yahoo!"/>
+    <x:hyperlink ref="A1" r:id="rId13"/>
+    <x:hyperlink ref="A2" r:id="rId14" tooltip="Click to go to Yahoo!"/>
     <x:hyperlink ref="A3" location="Hyperlinks!Test.xlsx" display="Link to a file - same folder"/>
-    <x:hyperlink ref="A4" r:id="rId16"/>
-    <x:hyperlink ref="A5" r:id="rId17"/>
+    <x:hyperlink ref="A4" r:id="rId15"/>
+    <x:hyperlink ref="A5" r:id="rId16"/>
     <x:hyperlink ref="A6" location="Hyperlinks!B1" display="Link to an address in this worksheet"/>
     <x:hyperlink ref="A7" location="'Second Sheet'!A1" display="Link to an address in another worksheet"/>
     <x:hyperlink ref="A8" location="Hyperlinks!B1:C2" tooltip="SquareBox" display="Link to a range in this worksheet"/>
-    <x:hyperlink ref="A9" r:id="rId18"/>
+    <x:hyperlink ref="A9" r:id="rId17"/>
     <x:hyperlink ref="A11" location="Hyperlinks!B1:C2" display="Odd looking link"/>
-    <x:hyperlink ref="A12" r:id="rId19"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>